<commit_message>
add runner of deploy
</commit_message>
<xml_diff>
--- a/deploy.xlsx
+++ b/deploy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="63">
   <si>
     <t xml:space="preserve">测试项目</t>
   </si>
@@ -2217,7 +2217,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2294,10 +2294,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2340,10 +2336,6 @@
     </xf>
     <xf numFmtId="164" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -2454,21 +2446,21 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="H42" activeCellId="0" sqref="H42:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.2148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.6222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.31111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.3888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="31.8481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.5037037037037"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2522,7 +2514,9 @@
       <c r="G2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="I2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2543,7 +2537,9 @@
       <c r="G3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="I3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2564,7 +2560,9 @@
       <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="H4" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="I4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2585,10 +2583,12 @@
       <c r="G5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="14"/>
+      <c r="H5" s="10" t="s">
+        <v>14</v>
+      </c>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" s="21" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" s="20" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -2608,8 +2608,10 @@
       <c r="G6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="20"/>
+      <c r="H6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
@@ -2629,8 +2631,10 @@
       <c r="G7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
+      <c r="H7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
@@ -2650,11 +2654,13 @@
       <c r="G8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="20"/>
+      <c r="H8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -2673,11 +2679,13 @@
       <c r="G9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="20"/>
+      <c r="H9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="14" t="s">
         <v>25</v>
       </c>
@@ -2694,11 +2702,13 @@
       <c r="G10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="20"/>
+      <c r="H10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="19"/>
     </row>
     <row r="11" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="14" t="s">
         <v>26</v>
       </c>
@@ -2715,11 +2725,13 @@
       <c r="G11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="20"/>
+      <c r="H11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="14" t="s">
@@ -2738,11 +2750,13 @@
       <c r="G12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="20"/>
+      <c r="H12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="14" t="s">
         <v>30</v>
       </c>
@@ -2759,11 +2773,13 @@
       <c r="G13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
+      <c r="H13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="19"/>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="23"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="14" t="s">
         <v>31</v>
       </c>
@@ -2780,11 +2796,13 @@
       <c r="G14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="20"/>
+      <c r="H14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="19"/>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="14" t="s">
@@ -2803,11 +2821,13 @@
       <c r="G15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="20"/>
+      <c r="H15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="14" t="s">
         <v>34</v>
       </c>
@@ -2824,11 +2844,13 @@
       <c r="G16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="20"/>
+      <c r="H16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="14" t="s">
         <v>31</v>
       </c>
@@ -2845,8 +2867,10 @@
       <c r="G17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="20"/>
+      <c r="H17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
@@ -2858,7 +2882,7 @@
       <c r="C18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E18" s="16" t="s">
@@ -2870,8 +2894,10 @@
       <c r="G18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="20"/>
+      <c r="H18" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
@@ -2881,7 +2907,7 @@
       <c r="C19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="16" t="s">
         <v>13</v>
       </c>
@@ -2891,8 +2917,10 @@
       <c r="G19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="20"/>
+      <c r="H19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
@@ -2902,7 +2930,7 @@
       <c r="C20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="24"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="16" t="s">
         <v>13</v>
       </c>
@@ -2912,8 +2940,10 @@
       <c r="G20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="20"/>
+      <c r="H20" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
@@ -2923,7 +2953,7 @@
       <c r="C21" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="16" t="s">
         <v>13</v>
       </c>
@@ -2933,8 +2963,10 @@
       <c r="G21" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
+      <c r="H21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
@@ -2944,7 +2976,7 @@
       <c r="C22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="24"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="16" t="s">
         <v>13</v>
       </c>
@@ -2954,8 +2986,10 @@
       <c r="G22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
+      <c r="H22" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
@@ -2967,7 +3001,7 @@
       <c r="C23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="24"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="16" t="s">
         <v>13</v>
       </c>
@@ -2977,8 +3011,10 @@
       <c r="G23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H23" s="19"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
@@ -2988,7 +3024,7 @@
       <c r="C24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="24"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="16" t="s">
         <v>13</v>
       </c>
@@ -2998,8 +3034,10 @@
       <c r="G24" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H24" s="19"/>
-      <c r="I24" s="20"/>
+      <c r="H24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
@@ -3009,7 +3047,7 @@
       <c r="C25" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="24"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="16" t="s">
         <v>13</v>
       </c>
@@ -3019,8 +3057,10 @@
       <c r="G25" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H25" s="19"/>
-      <c r="I25" s="20"/>
+      <c r="H25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
@@ -3030,7 +3070,7 @@
       <c r="C26" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="24"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="16" t="s">
         <v>13</v>
       </c>
@@ -3040,8 +3080,10 @@
       <c r="G26" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="20"/>
+      <c r="H26" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
@@ -3051,7 +3093,7 @@
       <c r="C27" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="24"/>
+      <c r="D27" s="23"/>
       <c r="E27" s="16" t="s">
         <v>13</v>
       </c>
@@ -3061,11 +3103,13 @@
       <c r="G27" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20"/>
+      <c r="H27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="19"/>
     </row>
     <row r="28" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="24" t="s">
         <v>46</v>
       </c>
       <c r="B28" s="14" t="s">
@@ -3074,7 +3118,7 @@
       <c r="C28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E28" s="16" t="s">
@@ -3086,18 +3130,20 @@
       <c r="G28" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="19"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="26"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="16" t="s">
         <v>13</v>
       </c>
@@ -3107,18 +3153,20 @@
       <c r="G29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="20"/>
+      <c r="H29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="19"/>
     </row>
     <row r="30" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="26"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="16" t="s">
         <v>13</v>
       </c>
@@ -3128,18 +3176,20 @@
       <c r="G30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="20"/>
+      <c r="H30" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="19"/>
     </row>
     <row r="31" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="16" t="s">
         <v>13</v>
       </c>
@@ -3149,18 +3199,20 @@
       <c r="G31" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="20"/>
+      <c r="H31" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="19"/>
     </row>
     <row r="32" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="14" t="s">
         <v>51</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="26"/>
+      <c r="D32" s="25"/>
       <c r="E32" s="16" t="s">
         <v>13</v>
       </c>
@@ -3170,18 +3222,20 @@
       <c r="G32" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="20"/>
+      <c r="H32" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="19"/>
     </row>
     <row r="33" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="26"/>
+      <c r="D33" s="25"/>
       <c r="E33" s="16" t="s">
         <v>13</v>
       </c>
@@ -3191,18 +3245,20 @@
       <c r="G33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="20"/>
+      <c r="H33" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="25"/>
+      <c r="A34" s="24"/>
       <c r="B34" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="26"/>
+      <c r="D34" s="25"/>
       <c r="E34" s="16" t="s">
         <v>13</v>
       </c>
@@ -3212,18 +3268,20 @@
       <c r="G34" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="20"/>
+      <c r="H34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="25"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="26"/>
+      <c r="D35" s="25"/>
       <c r="E35" s="16" t="s">
         <v>13</v>
       </c>
@@ -3233,18 +3291,20 @@
       <c r="G35" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="20"/>
+      <c r="H35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="19"/>
     </row>
     <row r="36" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="25"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="26"/>
+      <c r="D36" s="25"/>
       <c r="E36" s="16" t="s">
         <v>13</v>
       </c>
@@ -3254,18 +3314,20 @@
       <c r="G36" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="I36" s="20"/>
+      <c r="H36" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="19"/>
     </row>
     <row r="37" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="25"/>
+      <c r="A37" s="24"/>
       <c r="B37" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="26"/>
+      <c r="D37" s="25"/>
       <c r="E37" s="16" t="s">
         <v>13</v>
       </c>
@@ -3275,18 +3337,20 @@
       <c r="G37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="20"/>
+      <c r="H37" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="19"/>
     </row>
     <row r="38" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="26"/>
+      <c r="D38" s="25"/>
       <c r="E38" s="16" t="s">
         <v>13</v>
       </c>
@@ -3296,18 +3360,20 @@
       <c r="G38" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="20"/>
+      <c r="H38" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="19"/>
     </row>
     <row r="39" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="25"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="26"/>
+      <c r="D39" s="25"/>
       <c r="E39" s="16" t="s">
         <v>13</v>
       </c>
@@ -3317,18 +3383,20 @@
       <c r="G39" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="20"/>
+      <c r="H39" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="19"/>
     </row>
     <row r="40" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="25"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="26"/>
+      <c r="D40" s="25"/>
       <c r="E40" s="16" t="s">
         <v>13</v>
       </c>
@@ -3338,18 +3406,20 @@
       <c r="G40" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H40" s="19"/>
-      <c r="I40" s="20"/>
+      <c r="H40" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="19"/>
     </row>
     <row r="41" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="25"/>
+      <c r="A41" s="24"/>
       <c r="B41" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="26"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="16" t="s">
         <v>13</v>
       </c>
@@ -3359,18 +3429,20 @@
       <c r="G41" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="20"/>
+      <c r="H41" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="19"/>
     </row>
     <row r="42" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="25"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="26"/>
+      <c r="D42" s="25"/>
       <c r="E42" s="16" t="s">
         <v>13</v>
       </c>
@@ -3380,29 +3452,33 @@
       <c r="G42" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H42" s="19"/>
-      <c r="I42" s="20"/>
+      <c r="H42" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="19"/>
     </row>
     <row r="43" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="25"/>
-      <c r="B43" s="27" t="s">
+      <c r="A43" s="24"/>
+      <c r="B43" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="26"/>
-      <c r="E43" s="29" t="s">
+      <c r="C43" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="25"/>
+      <c r="E43" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="30" t="s">
+      <c r="F43" s="29" t="s">
         <v>14</v>
       </c>
       <c r="G43" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H43" s="31"/>
-      <c r="I43" s="32"/>
+      <c r="H43" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3427,7 +3503,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F43" type="none">
+    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F43 H2:H43" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>